<commit_message>
Enabling New Sanity to LogixalBox2
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
@@ -65,28 +65,28 @@
     <t>CSS</t>
   </si>
   <si>
+    <t>EleType1</t>
+  </si>
+  <si>
+    <t>EleType2</t>
+  </si>
+  <si>
+    <t>JSElement</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
     <t>CLICK_JS</t>
   </si>
   <si>
+    <t>EnableCertificate_GoTOPage</t>
+  </si>
+  <si>
+    <t>JS_ID</t>
+  </si>
+  <si>
     <t>EnableCertificate_MoreInfo</t>
-  </si>
-  <si>
-    <t>EnableCertificate_GoTOPage</t>
-  </si>
-  <si>
-    <t>EleType1</t>
-  </si>
-  <si>
-    <t>EleType2</t>
-  </si>
-  <si>
-    <t>JSElement</t>
-  </si>
-  <si>
-    <t>WAIT</t>
-  </si>
-  <si>
-    <t>JS_ID</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -550,22 +550,22 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -574,22 +574,22 @@
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -598,7 +598,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -712,18 +712,18 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -741,15 +741,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -946,6 +937,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
@@ -956,14 +956,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -980,4 +972,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>